<commit_message>
update data downlaods for reform with sources
</commit_message>
<xml_diff>
--- a/data/download/Alabama Prison Admissions and Population - 2007-2014.xlsx
+++ b/data/download/Alabama Prison Admissions and Population - 2007-2014.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EPelletier\Desktop\Plane Work\DOWNLOADABLE DATA FILES\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -32,11 +32,20 @@
   <si>
     <t>Alabama Prison Admissions and Standing Population - 2007-2014</t>
   </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>National Corrections Reporting Program</t>
+  </si>
+  <si>
+    <t>https://www.bjs.gov/index.cfm?ty=dcdetail&amp;iid=268</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,7 +627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -670,7 +679,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -864,7 +873,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -872,25 +881,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2007</v>
       </c>
@@ -912,7 +921,7 @@
         <v>26349</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -923,7 +932,7 @@
         <v>27304</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2009</v>
       </c>
@@ -934,7 +943,7 @@
         <v>27905</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2010</v>
       </c>
@@ -945,7 +954,7 @@
         <v>27684</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -956,7 +965,7 @@
         <v>27905</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -967,7 +976,7 @@
         <v>28069</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -978,7 +987,7 @@
         <v>27714</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -989,8 +998,28 @@
         <v>26969</v>
       </c>
     </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>